<commit_message>
Co-po mapping 2nd table
</commit_message>
<xml_diff>
--- a/14 15 PO and PSO.xlsx
+++ b/14 15 PO and PSO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raynf\OneDrive\Desktop\formfilling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B363FF85-2508-4164-B4E2-24020837B9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFB425F-1B1E-47E9-B1D5-F1496A23B737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>PO1</t>
   </si>
@@ -112,10 +112,16 @@
     <t>Use professional best engineering practices &amp; strategies for operation &amp; maintenance of mechanical systems &amp; processes.</t>
   </si>
   <si>
-    <t xml:space="preserve">heading:PROGRAM OUTCOMES [PO`s] .The students after successful completion of the course will acquire: </t>
-  </si>
-  <si>
-    <t>heading:PROGRAM SPECIFIC OUTCOMES [PSO's].At the end of the program graduates will be able to:</t>
+    <t xml:space="preserve">text:The students after successful completion of the course will acquire: </t>
+  </si>
+  <si>
+    <t>heading:PROGRAM SPECIFIC OUTCOMES [PSO's].</t>
+  </si>
+  <si>
+    <t>text:At the end of the program graduates will be able to:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heading:List of PROGRAM OUTCOMES [PO`s] </t>
   </si>
 </sst>
 </file>
@@ -462,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -477,7 +483,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -506,7 +512,9 @@
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -976,7 +984,9 @@
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>

</xml_diff>